<commit_message>
Se elimina todo de flyio para cambiar a heroku
</commit_message>
<xml_diff>
--- a/spec/files/properties/location_error.xlsx
+++ b/spec/files/properties/location_error.xlsx
@@ -26,7 +26,7 @@
     <t xml:space="preserve">tipo-propiedad</t>
   </si>
   <si>
-    <t xml:space="preserve">localización</t>
+    <t xml:space="preserve">localizacion</t>
   </si>
   <si>
     <t xml:space="preserve">Propio#pro-own</t>
@@ -437,7 +437,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>